<commit_message>
Q4 GDP Third Estimate
</commit_message>
<xml_diff>
--- a/data/auxilliary/haver_names.xlsx
+++ b/data/auxilliary/haver_names.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malcalakovalski/Documents/Projects/Fiscal-Impact-Measure/data/auxilliary/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malcalakovalski\Documents\Fiscal-Impact-Measure\data\auxilliary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A43BD41-ABA2-E544-9071-51676FF0B8EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C270298-FDD5-4888-8742-7687E4973A9E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="500" windowWidth="16800" windowHeight="19500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="122">
   <si>
     <t>code</t>
   </si>
@@ -385,6 +382,18 @@
   </si>
   <si>
     <t>state_subsidies</t>
+  </si>
+  <si>
+    <t>gfsubv</t>
+  </si>
+  <si>
+    <t>provider_relief_fund_grants</t>
+  </si>
+  <si>
+    <t>gftfpr</t>
+  </si>
+  <si>
+    <t>medicare_reimbursement_increase</t>
   </si>
 </sst>
 </file>
@@ -771,18 +780,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="221" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="221" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -790,7 +799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -798,7 +807,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -806,7 +815,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -814,7 +823,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -822,7 +831,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -830,7 +839,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -838,7 +847,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -846,7 +855,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -854,7 +863,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -862,7 +871,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -870,7 +879,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -878,7 +887,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -886,7 +895,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -894,7 +903,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -902,7 +911,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -910,7 +919,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -918,7 +927,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -926,7 +935,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -934,7 +943,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -942,7 +951,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -950,7 +959,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -958,7 +967,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -966,7 +975,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -974,7 +983,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -982,7 +991,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -990,7 +999,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -998,7 +1007,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1006,7 +1015,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1014,7 +1023,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1022,7 +1031,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -1030,7 +1039,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -1038,7 +1047,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -1046,7 +1055,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1054,7 +1063,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -1062,7 +1071,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -1070,7 +1079,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -1078,7 +1087,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -1086,7 +1095,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -1094,7 +1103,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -1102,7 +1111,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>43</v>
       </c>
@@ -1110,7 +1119,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -1118,7 +1127,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -1126,7 +1135,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -1134,7 +1143,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -1142,123 +1151,139 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
+        <v>120</v>
+      </c>
+      <c r="B46" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>51</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>52</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>53</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>54</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>55</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>69</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>68</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>118</v>
+      </c>
+      <c r="B54" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
         <v>56</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B55" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>57</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B56" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
         <v>58</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B57" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>59</v>
       </c>
-      <c r="B56" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="B58" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
         <v>62</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B59" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
         <v>60</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B60" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
         <v>61</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B61" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
         <v>66</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B62" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1268,12 +1293,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1494,15 +1516,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11C50A7A-072C-42B0-A807-112C623C860C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C7CC3BF-DF9F-4E15-B3E2-3F2BE52E9D01}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1527,10 +1553,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C7CC3BF-DF9F-4E15-B3E2-3F2BE52E9D01}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11C50A7A-072C-42B0-A807-112C623C860C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>